<commit_message>
JNG-3902 Use timestamp instead of time with hsqldb
</commit_message>
<xml_diff>
--- a/judo-tatami-asm2rdbms/model/RDBMS_Data_Types_Hsqldb.xlsx
+++ b/judo-tatami-asm2rdbms/model/RDBMS_Data_Types_Hsqldb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bence/Projects/judo-ng/runtime/judo-tatami-base/judo-tatami-asm2rdbms/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E570864-57AC-E74A-AA85-09F1EE94F177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72F0A2D-8627-C04D-8810-ACCEF3B13053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7540" yWindow="2440" windowWidth="28000" windowHeight="20180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12500" yWindow="4180" windowWidth="28000" windowHeight="20180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="57">
   <si>
     <t>Judo</t>
   </si>
@@ -190,14 +190,14 @@
     <t>org.joda.time.LocalTime</t>
   </si>
   <si>
-    <t>TIME</t>
+    <t>note: While HSQLDB has TIME type, jdbc driver returns values wihtout fractional part of seconds therefore TIMESTAMP is used with coercer to keep fractional part in resultset</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -213,6 +213,14 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -255,11 +263,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1019"/>
+  <dimension ref="A1:H1019"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -618,6 +629,7 @@
     <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1186,7 +1198,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>50</v>
       </c>
@@ -1205,7 +1217,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>51</v>
       </c>
@@ -1224,75 +1236,81 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G35" s="3">
         <v>93</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H35" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="G36" s="3">
         <v>93</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G37" s="3">
         <v>93</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="G38" s="3">
         <v>93</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="1"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1301,7 +1319,7 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="1"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1310,7 +1328,7 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="1"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1319,7 +1337,7 @@
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="1"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1328,7 +1346,7 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="1"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1337,7 +1355,7 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="1"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1346,7 +1364,7 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="1"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1355,7 +1373,7 @@
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1364,7 +1382,7 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -1373,7 +1391,7 @@
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
     </row>
-    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -10122,6 +10140,9 @@
       <c r="G1019" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H35:H38"/>
+  </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
   <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
OffsetDateTime to LocalDateTime transition
</commit_message>
<xml_diff>
--- a/judo-tatami-asm2rdbms/model/RDBMS_Data_Types_Hsqldb.xlsx
+++ b/judo-tatami-asm2rdbms/model/RDBMS_Data_Types_Hsqldb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bence/Projects/judo-ng/runtime/judo-tatami-base/judo-tatami-asm2rdbms/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72F0A2D-8627-C04D-8810-ACCEF3B13053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF27D610-4E41-7349-B29B-A007292C7130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12500" yWindow="4180" windowWidth="28000" windowHeight="20180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13220" yWindow="5420" windowWidth="28000" windowHeight="20180" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="1" r:id="rId1"/>
@@ -617,7 +617,7 @@
   <dimension ref="A1:H1019"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.6640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -734,10 +734,10 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G6" s="3">
-        <v>2014</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -768,10 +768,10 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G8" s="3">
-        <v>2014</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -785,10 +785,10 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G9" s="3">
-        <v>2014</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -802,10 +802,10 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G10" s="3">
-        <v>2014</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -836,10 +836,10 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G12" s="3">
-        <v>2014</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>